<commit_message>
Finished optimization in latex report
</commit_message>
<xml_diff>
--- a/portfolio-matrices/bohbohboh.xlsx
+++ b/portfolio-matrices/bohbohboh.xlsx
@@ -471,19 +471,19 @@
         <v>43465</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1674303660754783</v>
+        <v>0.167429060537152</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1929983144548651</v>
+        <v>0.1929990211824646</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2008565642845515</v>
+        <v>0.2008582840095177</v>
       </c>
       <c r="E2" t="n">
-        <v>0.252181823230986</v>
+        <v>0.2521840170226298</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1865329319541189</v>
+        <v>0.1865296172482358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>